<commit_message>
Added links to readings.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3A994-4CF7-8648-B270-652F4EDE96D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3ABE40-B59C-CD47-8D80-DDB22F696630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="1740" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -152,39 +152,21 @@
     <t>Introduction to R, Rstudio, and the course</t>
   </si>
   <si>
-    <t>IMStat Chapter 1</t>
-  </si>
-  <si>
     <t>Data Visualization</t>
   </si>
   <si>
-    <t>[R4DS Chapter 3[(https://r4ds.had.co.nz/data-visualisation.html)</t>
-  </si>
-  <si>
     <t>Introduction to Data</t>
   </si>
   <si>
-    <t>IMStat Chapters 2 and 3</t>
-  </si>
-  <si>
     <t>Bivariate Regression</t>
   </si>
   <si>
-    <t>IMStat Chapter 7</t>
-  </si>
-  <si>
-    <t>IMStat Chapter 8</t>
-  </si>
-  <si>
     <t>Multiple Regression</t>
   </si>
   <si>
     <t>Maximum Likelihood Estimation and Logistic Regression</t>
   </si>
   <si>
-    <t>IMStat Chapter 9</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
@@ -197,19 +179,10 @@
     <t>Inference for Categorical Data</t>
   </si>
   <si>
-    <t>IMStat Chapters 16, 17, and 18</t>
-  </si>
-  <si>
     <t>Inference for Numerical Data</t>
   </si>
   <si>
-    <t>IMStat Chapters 19, 20, and 21</t>
-  </si>
-  <si>
     <t>ANOVA</t>
-  </si>
-  <si>
-    <t>IMStat Chapter 22</t>
   </si>
   <si>
     <t>[Intro to Data Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/02_intro_to_data.zip)</t>
@@ -235,6 +208,33 @@
   <si>
     <t>[Formative Assessment](https://forms.gle/PJZSMSYQsjYAAvY27)  
 [Intro to R Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/01_intro_to_r.zip)</t>
+  </si>
+  <si>
+    <t>IMStat Chapters [2](https://openintro-ims.netlify.app/data-design) and [3](https://openintro-ims.netlify.app/data-applications)</t>
+  </si>
+  <si>
+    <t>IMStat [Chapter 1](https://openintro-ims.netlify.app/data-hello)</t>
+  </si>
+  <si>
+    <t>IMStat [Chapter 7](https://openintro-ims.netlify.app/model-slr)</t>
+  </si>
+  <si>
+    <t>IMStat [Chapter 8](https://openintro-ims.netlify.app/model-mlr)</t>
+  </si>
+  <si>
+    <t>IMStat [Chapter 9](https://openintro-ims.netlify.app/model-logistic)</t>
+  </si>
+  <si>
+    <t>IMStat Chapters [16](https://openintro-ims.netlify.app/inference-one-prop), [17](https://openintro-ims.netlify.app/inference-two-props), and [18](https://openintro-ims.netlify.app/inference-tables)</t>
+  </si>
+  <si>
+    <t>IMStat Chapters [19](https://openintro-ims.netlify.app/inference-one-mean), [20](https://openintro-ims.netlify.app/inference-two-means), and [21](https://openintro-ims.netlify.app/inference-paired-means)</t>
+  </si>
+  <si>
+    <t>IMStat [Chapter 22](https://openintro-ims.netlify.app/inference-many-means)</t>
+  </si>
+  <si>
+    <t>R4DS [Chapter 3](https://r4ds.had.co.nz/data-visualisation.html)</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,10 +1025,10 @@
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1039,13 +1039,13 @@
         <v>45319</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1056,10 +1056,10 @@
         <v>45326</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1070,13 +1070,13 @@
         <v>45340</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1087,13 +1087,13 @@
         <v>45340</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1104,10 +1104,10 @@
         <v>45347</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,13 +1118,13 @@
         <v>45354</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
         <v>45361</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,10 +1146,10 @@
         <v>45368</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1160,10 +1160,10 @@
         <v>45375</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,10 +1174,10 @@
         <v>45382</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>45389</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>45396</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>45403</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated readme with link to slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485AEC49-E81B-0441-8FB7-C03F2CC90A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180F913A-1977-1441-A17F-F51F0A6FE221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="7780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="200" yWindow="1740" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -149,9 +149,6 @@
     <t>Assignments</t>
   </si>
   <si>
-    <t>Introduction to R, Rstudio, and the course</t>
-  </si>
-  <si>
     <t>Data Visualization</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   <si>
     <t>[Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/08_simple_regression.zip)  
 Homework: TBD</t>
+  </si>
+  <si>
+    <t>[Introduction to R, Rstudio, and the course](https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-01-16-Intro_to_Course.pdf)</t>
   </si>
 </sst>
 </file>
@@ -993,10 +993,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,7 +1010,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1042,13 +1042,13 @@
         <v>45312</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1062,13 +1062,13 @@
         <v>45319</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1082,10 +1082,10 @@
         <v>45326</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1099,13 +1099,13 @@
         <v>45340</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1119,13 +1119,13 @@
         <v>45340</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1139,13 +1139,13 @@
         <v>45347</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1159,13 +1159,13 @@
         <v>45354</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>45361</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1193,10 +1193,10 @@
         <v>45368</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1210,10 +1210,10 @@
         <v>45375</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1227,10 +1227,10 @@
         <v>45382</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1244,7 +1244,7 @@
         <v>45389</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1258,7 +1258,7 @@
         <v>45396</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1272,7 +1272,7 @@
         <v>45403</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated schedule and labs.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0059B5D8-ED5C-214A-AE3D-F70BD7977597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB644EA-0ACE-654D-B7AF-ED6E574FE0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="5160" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -147,12 +147,6 @@
   </si>
   <si>
     <t>Assignments</t>
-  </si>
-  <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Introduction to Data</t>
   </si>
   <si>
     <t>Bivariate Regression</t>
@@ -195,9 +189,6 @@
 [Intro to R Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/01_intro_to_r.zip)</t>
   </si>
   <si>
-    <t>IMStat Chapters [2](https://openintro-ims.netlify.app/data-design) and [3](https://openintro-ims.netlify.app/data-applications)</t>
-  </si>
-  <si>
     <t>IMStat [Chapter 1](https://openintro-ims.netlify.app/data-hello)</t>
   </si>
   <si>
@@ -219,28 +210,13 @@
     <t>IMStat [Chapter 22](https://openintro-ims.netlify.app/inference-many-means)</t>
   </si>
   <si>
-    <t>R4DS [Chapter 3](https://r4ds.had.co.nz/data-visualisation.html)</t>
-  </si>
-  <si>
     <t>Week</t>
-  </si>
-  <si>
-    <t>Probability Lab  
-Homework: TBD</t>
-  </si>
-  <si>
-    <t>[Multiple Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/09_multiple_regression.zip)  
-Homework: TBD</t>
   </si>
   <si>
     <t>Logistic Regression Lab
 Homework: TBD</t>
   </si>
   <si>
-    <t>[Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/08_simple_regression.zip)  
-Homework: TBD</t>
-  </si>
-  <si>
     <t>Introduction to R, Rstudio, and the course</t>
   </si>
   <si>
@@ -249,6 +225,40 @@
   <si>
     <t>[Intro to Data Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/02_intro_to_data.zip)  
 Homework: 1.4, 1.10, 2.4, 2.16, 2.24</t>
+  </si>
+  <si>
+    <t>Introduction to Data and Data Visualization</t>
+  </si>
+  <si>
+    <t>IMStat Chapters [2](https://openintro-ims.netlify.app/data-design) and [3](https://openintro-ims.netlify.app/data-applications)  
+R4DS [Chapter 3](https://r4ds.had.co.nz/data-visualisation.html)</t>
+  </si>
+  <si>
+    <t>IMStat Chapters [11](https://openintro-ims.netlify.app/foundations-randomization), [12](https://openintro-ims.netlify.app/foundations-bootstrapping), and [13](https://openintro-ims.netlify.app/foundations-mathematical)</t>
+  </si>
+  <si>
+    <t>[Probability Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/03_probability.zip)  
+Homework: TBD</t>
+  </si>
+  <si>
+    <t>[Multiple Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/08_multiple_regression.zip)  
+Homework: TBD</t>
+  </si>
+  <si>
+    <t>[Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/07_simple_linear_regression.zip)  
+Homework: TBD</t>
+  </si>
+  <si>
+    <t>[Foundation for Inference Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/11_foundations_for_inference.zip) (*note there are two parts*)</t>
+  </si>
+  <si>
+    <t>[Inference for Categorical Data Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/16_inference_for_categorial_data.zip)</t>
+  </si>
+  <si>
+    <t>[Inference for Numerical Data Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/19_inference_for_numerical_data.zip)</t>
+  </si>
+  <si>
+    <t>[ANOVA Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/22_ANOVA.zip)</t>
   </si>
 </sst>
 </file>
@@ -650,7 +660,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,24 +1006,24 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
-    <col min="6" max="6" width="177.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="50.33203125" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1045,16 +1055,16 @@
         <v>45312</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -1068,13 +1078,13 @@
         <v>45319</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1087,14 +1097,8 @@
       <c r="C4" s="11">
         <v>45326</v>
       </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1105,13 +1109,13 @@
         <v>45340</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1125,16 +1129,16 @@
         <v>45340</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1145,16 +1149,16 @@
         <v>45347</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1168,13 +1172,13 @@
         <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1185,10 +1189,16 @@
         <v>45361</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1199,13 +1209,16 @@
         <v>45368</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1216,13 +1229,16 @@
         <v>45375</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1233,10 +1249,13 @@
         <v>45382</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1250,7 +1269,7 @@
         <v>45389</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1264,7 +1283,7 @@
         <v>45396</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1278,7 +1297,7 @@
         <v>45403</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added logistic regression lab.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BB1370-65F6-DF41-BD70-C128855AE6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA058E4-9601-1342-BE00-1C78D2F73A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -213,10 +213,6 @@
     <t>Week</t>
   </si>
   <si>
-    <t>Logistic Regression Lab
-Homework: TBD</t>
-  </si>
-  <si>
     <t>Introduction to R, Rstudio, and the course</t>
   </si>
   <si>
@@ -265,6 +261,10 @@
   </si>
   <si>
     <t>https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-01-23-Intro_to_Data.pdf</t>
+  </si>
+  <si>
+    <t>[Logistic Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/09_logistic_regression.zip)
+Homework: TBD</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1012,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,10 +1061,10 @@
         <v>45312</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -1084,16 +1084,16 @@
         <v>45319</v>
       </c>
       <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>51</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1153,10 +1153,10 @@
         <v>52</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,7 @@
         <v>45354</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1204,10 +1204,10 @@
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1227,7 +1227,7 @@
         <v>54</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1247,7 +1247,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1267,7 +1267,7 @@
         <v>56</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added slides. Updated schedule.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04999D4D-0F69-9C47-B3DF-FA6C51262128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF006E5C-3E7E-8F4E-9F86-BC3906BEE55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="1560" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,6 @@
     <t>[ANOVA Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/22_ANOVA.zip)</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-01-23-Intro_to_Data.pdf</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   <si>
     <t>[Probability Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/03_probability.zip)  
 Homework (Note these are from the OpenIntro Statistics book): 3.7, 3.17, 3.25, 3.33, 3.37</t>
+  </si>
+  <si>
+    <t>There will be no class on February 27th.</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1012,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,7 +1087,7 @@
         <v>61</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>62</v>
@@ -1113,7 +1113,7 @@
         <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,7 @@
         <v>45354</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added slides and project.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FAC1B9-87A3-D64E-86B4-217F75673371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA83FBE-83D4-CC4B-BAD7-7EEEDE8B9EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="7740" windowWidth="31820" windowHeight="19160" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -265,12 +265,21 @@
 Homework: 7.4, 7.8, 7.20, 7.22</t>
   </si>
   <si>
-    <t>[Multiple Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/08_multiple_regression.zip)   
-Homework: TBD</t>
-  </si>
-  <si>
     <t>[Logistic Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/09_logistic_regression.zip)  
 Homework: 9.2, 9.4, 9.6</t>
+  </si>
+  <si>
+    <t>https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-02-13-Logistic_Regression.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-02-20-Multiple_Regression.pdf</t>
+  </si>
+  <si>
+    <t>[Multiple Regression Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/08_multiple_regression.zip)   
+Homework: 8.4, 8.6, 8.10</t>
+  </si>
+  <si>
+    <t>[Data Project Proposal](https://github.com/jbryer/DAV5300-2024-Spring/tree/master/project/data_project.md)</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1030,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,11 +1170,14 @@
       <c r="D6" t="s">
         <v>39</v>
       </c>
+      <c r="E6" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="F6" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1181,14 +1193,17 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
+      <c r="E7" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="F7" t="s">
         <v>52</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1200,6 +1215,9 @@
       </c>
       <c r="D8" t="s">
         <v>70</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1359,6 +1377,8 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{772AC442-940E-AE41-8A04-291AD6FE3798}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{1962F67A-F81F-7B45-933E-71F665989C1E}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{EADC0DDC-DA8B-B443-9441-3707D719DF85}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{E84C4455-2353-9B4C-A862-2CA9D73A0C70}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{B68EDD1F-9EFA-9F42-83DC-347D5F304B3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added slides and homework.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0674DB9B-D1A1-2A40-A59D-C7E07D7C5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F86650-186C-5A44-A5C1-4EF522E7C3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Foundation for Inference / Central Limit Theorem</t>
-  </si>
-  <si>
-    <t>Introduction to Predictive Modeling</t>
   </si>
   <si>
     <t>Bayesian Analysis</t>
@@ -233,9 +230,6 @@
     <t>IMStat Chapters [11](https://openintro-ims.netlify.app/foundations-randomization), [12](https://openintro-ims.netlify.app/foundations-bootstrapping), and [13](https://openintro-ims.netlify.app/foundations-mathematical)</t>
   </si>
   <si>
-    <t>[Foundation for Inference Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/11_foundations_for_inference.zip) (*note there are two parts*)</t>
-  </si>
-  <si>
     <t>[Inference for Categorical Data Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/16_inference_for_categorial_data.zip)</t>
   </si>
   <si>
@@ -280,6 +274,17 @@
   </si>
   <si>
     <t>[Data Project Proposal](https://github.com/jbryer/DAV5300-2024-Spring/tree/master/project/data_project.md)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>https://github.com/jbryer/DAV5300-2024-Spring/blob/master/slides/2024-03-05-Foundation_for_Inference.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Foundation for Inference Lab](https://github.com/jbryer/DAV5300-2024-Spring/raw/master/labs/11_foundations_for_inference.zip) (*note there are two parts*)  
+Homework: 11.8, 12.8, 13.2
+</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1032,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,7 +1049,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1076,16 +1081,16 @@
         <v>45312</v>
       </c>
       <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -1099,16 +1104,16 @@
         <v>45319</v>
       </c>
       <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -1125,13 +1130,13 @@
         <v>40</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1148,13 +1153,13 @@
         <v>37</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1171,13 +1176,13 @@
         <v>39</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1194,13 +1199,13 @@
         <v>38</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1214,13 +1219,13 @@
         <v>45354</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1233,11 +1238,14 @@
       <c r="D9" t="s">
         <v>46</v>
       </c>
+      <c r="E9" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1254,10 +1262,10 @@
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1274,10 +1282,10 @@
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1294,10 +1302,10 @@
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1311,7 +1319,7 @@
         <v>45389</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1325,7 +1333,7 @@
         <v>45396</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,6 +1387,7 @@
     <hyperlink ref="E5" r:id="rId4" xr:uid="{EADC0DDC-DA8B-B443-9441-3707D719DF85}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{E84C4455-2353-9B4C-A862-2CA9D73A0C70}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{B68EDD1F-9EFA-9F42-83DC-347D5F304B3D}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{2F300788-00F3-124F-8BD8-F4BA354F8149}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>